<commit_message>
update ichthyo div data
</commit_message>
<xml_diff>
--- a/data-raw/NEFSCIchthyoplankton_v3_7_v2019.xlsx
+++ b/data-raw/NEFSCIchthyoplankton_v3_7_v2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwalsh/NEFSC larval samples/CombinedData/v3_7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09247E7-68E6-FB4F-89BF-6124D22F1069}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E2CBE-2D3D-A440-BAFD-A889898BB38F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{AE633ECA-40DE-1C41-B7FC-1DC3BECD58F9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{AE633ECA-40DE-1C41-B7FC-1DC3BECD58F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ichthyoplankton Taxa" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="116">
   <si>
     <t>Year</t>
   </si>
@@ -749,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CB16FA-2937-924D-B4F0-EC8A56CFA8AC}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1273,9 +1273,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB19F377-8BB2-624D-8145-B7DAD3DB9D49}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -1696,12 +1698,12 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>2.2032940720675498</v>
+        <v>2.20353217928117</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>1999</v>
+        <v>2019</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>59</v>
@@ -1710,18 +1712,18 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22">
-        <v>0.953180798659644</v>
+        <v>2.1644707676561499</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>59</v>
@@ -1736,12 +1738,12 @@
         <v>5</v>
       </c>
       <c r="F23">
-        <v>1.7186384848318901</v>
+        <v>0.953180798659644</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>59</v>
@@ -1756,12 +1758,12 @@
         <v>5</v>
       </c>
       <c r="F24">
-        <v>2.0099489651570002</v>
+        <v>1.7186384848318901</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>59</v>
@@ -1776,12 +1778,12 @@
         <v>5</v>
       </c>
       <c r="F25">
-        <v>1.86712329301817</v>
+        <v>2.0099489651570002</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>59</v>
@@ -1796,12 +1798,12 @@
         <v>5</v>
       </c>
       <c r="F26">
-        <v>2.2190713181937798</v>
+        <v>1.86712329301817</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>59</v>
@@ -1816,12 +1818,12 @@
         <v>5</v>
       </c>
       <c r="F27">
-        <v>1.58523211889477</v>
+        <v>2.2190713181937798</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>59</v>
@@ -1836,12 +1838,12 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>1.83781990475627</v>
+        <v>1.58523211889477</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>59</v>
@@ -1856,12 +1858,12 @@
         <v>5</v>
       </c>
       <c r="F29">
-        <v>2.2736607734929302</v>
+        <v>1.83781990475627</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>59</v>
@@ -1876,12 +1878,12 @@
         <v>5</v>
       </c>
       <c r="F30">
-        <v>0.80185571950397305</v>
+        <v>2.2736607734929302</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>59</v>
@@ -1896,12 +1898,12 @@
         <v>5</v>
       </c>
       <c r="F31">
-        <v>0.78163387698259601</v>
+        <v>0.80185571950397305</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>59</v>
@@ -1916,12 +1918,12 @@
         <v>5</v>
       </c>
       <c r="F32">
-        <v>2.03189819099219</v>
+        <v>0.78163387698259601</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>59</v>
@@ -1936,12 +1938,12 @@
         <v>5</v>
       </c>
       <c r="F33">
-        <v>2.0948832890626798</v>
+        <v>2.03189819099219</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>59</v>
@@ -1956,12 +1958,12 @@
         <v>5</v>
       </c>
       <c r="F34">
-        <v>1.7587995301359101</v>
+        <v>2.0948832890626798</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>59</v>
@@ -1976,12 +1978,12 @@
         <v>5</v>
       </c>
       <c r="F35">
-        <v>2.2952788471172099</v>
+        <v>1.7587995301359101</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>59</v>
@@ -1996,12 +1998,12 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>1.9974103699685599</v>
+        <v>2.2952788471172099</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>59</v>
@@ -2016,12 +2018,12 @@
         <v>5</v>
       </c>
       <c r="F37">
-        <v>1.5535218818854999</v>
+        <v>1.9974103699685599</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>59</v>
@@ -2036,12 +2038,12 @@
         <v>5</v>
       </c>
       <c r="F38">
-        <v>2.0575666441182698</v>
+        <v>1.5535218818854999</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>59</v>
@@ -2056,12 +2058,12 @@
         <v>5</v>
       </c>
       <c r="F39">
-        <v>2.07657227799915</v>
+        <v>2.0575666441182698</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>59</v>
@@ -2076,12 +2078,12 @@
         <v>5</v>
       </c>
       <c r="F40">
-        <v>1.9426549688914201</v>
+        <v>2.07657227799915</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>59</v>
@@ -2096,12 +2098,12 @@
         <v>5</v>
       </c>
       <c r="F41">
-        <v>2.0694991724249698</v>
+        <v>1.9426549688914201</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>1999</v>
+        <v>2018</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>59</v>
@@ -2110,18 +2112,18 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42">
-        <v>2.2773581889587899</v>
+        <v>2.0695966627581401</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>2000</v>
+        <v>2019</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>59</v>
@@ -2130,18 +2132,18 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43">
-        <v>1.79262114622353</v>
+        <v>1.93673233663968</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>59</v>
@@ -2156,12 +2158,12 @@
         <v>5</v>
       </c>
       <c r="F44">
-        <v>2.1162296671332701</v>
+        <v>2.2773581889587899</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>59</v>
@@ -2176,12 +2178,12 @@
         <v>5</v>
       </c>
       <c r="F45">
-        <v>2.3616977925468001</v>
+        <v>1.79262114622353</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>59</v>
@@ -2196,12 +2198,12 @@
         <v>5</v>
       </c>
       <c r="F46">
-        <v>1.4620638538459001</v>
+        <v>2.1162296671332701</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>59</v>
@@ -2216,12 +2218,12 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>1.7424912417337901</v>
+        <v>2.3616977925468001</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>59</v>
@@ -2236,12 +2238,12 @@
         <v>5</v>
       </c>
       <c r="F48">
-        <v>1.99949717344967</v>
+        <v>1.4620638538459001</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>59</v>
@@ -2256,12 +2258,12 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <v>2.1749223880627202</v>
+        <v>1.7424912417337901</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>59</v>
@@ -2276,12 +2278,12 @@
         <v>5</v>
       </c>
       <c r="F50">
-        <v>2.1250134746903999</v>
+        <v>1.99949717344967</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>59</v>
@@ -2296,12 +2298,12 @@
         <v>5</v>
       </c>
       <c r="F51">
-        <v>1.8382406840057699</v>
+        <v>2.1749223880627202</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>59</v>
@@ -2316,12 +2318,12 @@
         <v>5</v>
       </c>
       <c r="F52">
-        <v>1.77017086236796</v>
+        <v>2.1250134746903999</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>59</v>
@@ -2336,12 +2338,12 @@
         <v>5</v>
       </c>
       <c r="F53">
-        <v>2.1912922562933699</v>
+        <v>1.8382406840057699</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>59</v>
@@ -2356,12 +2358,12 @@
         <v>5</v>
       </c>
       <c r="F54">
-        <v>2.0516064959836502</v>
+        <v>1.77017086236796</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>59</v>
@@ -2376,12 +2378,12 @@
         <v>5</v>
       </c>
       <c r="F55">
-        <v>1.7892832331287101</v>
+        <v>2.1912922562933699</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>59</v>
@@ -2396,12 +2398,12 @@
         <v>5</v>
       </c>
       <c r="F56">
-        <v>2.1969654976724602</v>
+        <v>2.0516064959836502</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>59</v>
@@ -2416,12 +2418,12 @@
         <v>5</v>
       </c>
       <c r="F57">
-        <v>1.7249140146911399</v>
+        <v>1.7892832331287101</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>59</v>
@@ -2436,12 +2438,12 @@
         <v>5</v>
       </c>
       <c r="F58">
-        <v>1.8871028619130401</v>
+        <v>2.1969654976724602</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>59</v>
@@ -2455,10 +2457,13 @@
       <c r="E59" t="s">
         <v>5</v>
       </c>
+      <c r="F59">
+        <v>1.7249140146911399</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>59</v>
@@ -2473,12 +2478,12 @@
         <v>5</v>
       </c>
       <c r="F60">
-        <v>1.5338774971665099</v>
+        <v>1.8871028619130401</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>59</v>
@@ -2493,7 +2498,67 @@
         <v>5</v>
       </c>
       <c r="F61">
-        <v>2.0625959735925399</v>
+        <v>0.37327561959218702</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>2017</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62">
+        <v>1.5338774971665099</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>2018</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63">
+        <v>2.0902600976740402</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>2019</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>1.3276940604644001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>